<commit_message>
action-mode optimizations, beginnings of new copy/move routine
</commit_message>
<xml_diff>
--- a/WebAusleser.xlsx
+++ b/WebAusleser.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\har\Dropbox\WebAusleser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\Git\WebAusleser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -514,10 +514,10 @@
     <t>list_flag</t>
   </si>
   <si>
-    <t>wenn parent_id=-1, dann normaler schritt, sonst unterschritt zu step_id von if/for*/doloop</t>
-  </si>
-  <si>
     <t>wenn unterschritt-parameter, dann steht im value eine step_id, die als parent_id die step_id dieses unterschritt-parameters hat</t>
+  </si>
+  <si>
+    <t>wenn parent_id=-1, dann normaler schritt, sonst unterschritt zu param_id von if/for*/doloop</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>160</v>
       </c>
       <c r="H14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
main development of move and copy functionality
</commit_message>
<xml_diff>
--- a/WebAusleser.xlsx
+++ b/WebAusleser.xlsx
@@ -514,10 +514,10 @@
     <t>list_flag</t>
   </si>
   <si>
-    <t>wenn unterschritt-parameter, dann steht im value eine step_id, die als parent_id die step_id dieses unterschritt-parameters hat</t>
-  </si>
-  <si>
     <t>wenn parent_id=-1, dann normaler schritt, sonst unterschritt zu param_id von if/for*/doloop</t>
+  </si>
+  <si>
+    <t>wenn unterschritt-parameter, dann steht im value z. B. "then" oder "else" und hat als parent_id die step_id dieses unterschritt-parameters hat</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>160</v>
       </c>
       <c r="H14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
move and copy of if-then-else steps
</commit_message>
<xml_diff>
--- a/WebAusleser.xlsx
+++ b/WebAusleser.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="164">
   <si>
     <t>ActionBar</t>
   </si>
@@ -518,6 +518,9 @@
   </si>
   <si>
     <t>wenn unterschritt-parameter, dann steht im value z. B. "then" oder "else" und hat als parent_id die step_id dieses unterschritt-parameters hat</t>
+  </si>
+  <si>
+    <t>parental_flag</t>
   </si>
 </sst>
 </file>
@@ -1151,12 +1154,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1170,12 +1173,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1188,16 +1191,16 @@
       <c r="D6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1216,21 +1219,21 @@
       <c r="F10" t="s">
         <v>104</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1249,7 +1252,10 @@
       <c r="F14" t="s">
         <v>160</v>
       </c>
-      <c r="H14" t="s">
+      <c r="G14" t="s">
+        <v>163</v>
+      </c>
+      <c r="I14" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>